<commit_message>
updated GIM and DB to provide the information necessary for the RIA app
</commit_message>
<xml_diff>
--- a/docs/DB_DDL_helper_template.xlsx
+++ b/docs/DB_DDL_helper_template.xlsx
@@ -737,7 +737,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="272">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -1503,6 +1503,57 @@
   </si>
   <si>
     <t>A comma-delimited list of project resources and associated highest version number that have been implemented by the project.  If the current version implemented in the project is the same as the current version of the resource the project name is preceded by a "(CV)" prefix to indicate it is the current version and if not the "(UA)" prefix is used to indicate there is an update available</t>
+  </si>
+  <si>
+    <t>RES_NAME_CD_LIST</t>
+  </si>
+  <si>
+    <t>NUM_RES</t>
+  </si>
+  <si>
+    <t>IMPL_RES_CD_LIST</t>
+  </si>
+  <si>
+    <t>PRI_PROJ_RES_TAG_MAX_SUM_ALL_V</t>
+  </si>
+  <si>
+    <t>A comma-delimited list of project resources and associated highest version number that are associated with the project</t>
+  </si>
+  <si>
+    <t>The number of associated resources with the project</t>
+  </si>
+  <si>
+    <t>A comma-delimited list of project resources and associated highest version number that have been implemented by the project.  If the current version implemented in the project is the same as the current version of the resource the project name is preceded by a "*CV" prefix to indicate it is the current version and if not the "*UA" prefix is used to indicate there is an update available</t>
+  </si>
+  <si>
+    <t>ASSOC_PROJ_BR_LIST</t>
+  </si>
+  <si>
+    <t>ASSOC_PROJ_LINK_BR_LIST</t>
+  </si>
+  <si>
+    <t>RES_DESC</t>
+  </si>
+  <si>
+    <t>RES_DEMO_URL</t>
+  </si>
+  <si>
+    <t>PRI_RES_PROJ_TAG_MAX_SUM_ALL_V</t>
+  </si>
+  <si>
+    <t>A comma-delimited list of projects and associated highest version number that have implemented the given resource.  If the current version implemented is the same as the current version of the resource the project name is preceded by a "*CV" prefix to indicate it is the current version and if not the "*UA" prefix is used to indicate there is an update available</t>
+  </si>
+  <si>
+    <t>A web line-break-delimited (&lt;BR&gt;) list of projects and associated highest version number that have implemented the given resource.  If the current version implemented is the same as the current version of the resource the project name is preceded by a "*CV" prefix to indicate it is the current version and if not the "*UA" prefix is used to indicate there is an update available</t>
+  </si>
+  <si>
+    <t>A web line-break-delimited (&lt;BR&gt;) list of projects and associated highest version number in a formatted hyperlink with a relative path to the given Resource Inventory App project that has implemented the given resource.  If the current version implemented is the same as the current version of the resource the project name is preceded by a "*CV" prefix to indicate it is the current version and if not the "*UA" prefix is used to indicate there is an update available</t>
+  </si>
+  <si>
+    <t>The description for the project resource</t>
+  </si>
+  <si>
+    <t>The live demonstration URL for the project resource</t>
   </si>
 </sst>
 </file>
@@ -4509,8 +4560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2806"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C253" sqref="C253"/>
+    <sheetView tabSelected="1" topLeftCell="A334" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D350" sqref="D350:D385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7600,7 +7651,7 @@
         <v>82</v>
       </c>
       <c r="D246" s="22" t="str">
-        <f t="shared" ref="D246:D297" si="6">CONCATENATE("COMMENT ON COLUMN ",A246, ".", B246, " IS '", SUBSTITUTE(C246, "'", "''"), "';")</f>
+        <f t="shared" ref="D246:D309" si="6">CONCATENATE("COMMENT ON COLUMN ",A246, ".", B246, " IS '", SUBSTITUTE(C246, "'", "''"), "';")</f>
         <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_V.PROJ_ID IS 'Primary key for the PRI_PROJ table';</v>
       </c>
     </row>
@@ -8367,6 +8418,306 @@
       <c r="D297" s="22" t="str">
         <f t="shared" si="6"/>
         <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_V.RES_TYPE_DESC IS 'Description for the given Resource Type';</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A298" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B298" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C298" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D298" s="22" t="str">
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.PROJ_ID IS 'Primary key for the PRI_PROJ table';</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A299" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B299" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C299" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D299" s="22" t="str">
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.PROJ_NAME IS 'Name of the project';</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A300" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B300" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="C300" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="D300" s="22" t="str">
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.RES_NAME_CD_LIST IS 'A comma-delimited list of project resources and associated highest version number that are associated with the project';</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A301" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B301" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="C301" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="D301" s="22" t="str">
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.NUM_RES IS 'The number of associated resources with the project';</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A302" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B302" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="C302" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="D302" s="22" t="str">
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.CURR_VERS_COUNT IS 'The number of implemented resources that have been implemented by the project that are the same as the current version of the resource';</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A303" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B303" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="C303" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="D303" s="22" t="str">
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.OLD_VERS_COUNT IS 'The number of implemented resources that have been implemented by the project that are not the same as the current version of the resource';</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A304" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B304" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C304" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="D304" s="22" t="str">
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.TOTAL_IMPL_RES IS 'The total number of project resources that have been implemented in the given project';</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A305" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B305" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="C305" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="D305" s="22" t="str">
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.IMPL_RES_CD_LIST IS 'A comma-delimited list of project resources and associated highest version number that have been implemented by the project.  If the current version implemented in the project is the same as the current version of the resource the project name is preceded by a "*CV" prefix to indicate it is the current version and if not the "*UA" prefix is used to indicate there is an update available';</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A306" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B306" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C306" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D306" s="22" t="str">
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.VC_PROJ_ID IS 'Unique numeric ID of the project in the given version control system';</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A307" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B307" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C307" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D307" s="22" t="str">
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.PROJ_NAME IS 'Name of the project';</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A308" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B308" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C308" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D308" s="22" t="str">
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.PROJ_DESC IS 'Description of the project';</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A309" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B309" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C309" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D309" s="22" t="str">
+        <f t="shared" si="6"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.SSH_URL IS 'SSH URL for the project';</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A310" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B310" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C310" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D310" s="22" t="str">
+        <f t="shared" ref="D310:D317" si="7">CONCATENATE("COMMENT ON COLUMN ",A310, ".", B310, " IS '", SUBSTITUTE(C310, "'", "''"), "';")</f>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.HTTP_URL IS 'HTTP URL for the project';</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A311" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B311" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C311" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D311" s="22" t="str">
+        <f t="shared" si="7"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.README_URL IS 'Readme URL for the project';</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A312" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B312" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C312" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D312" s="22" t="str">
+        <f t="shared" si="7"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.AVATAR_URL IS 'Avatar URL for the project';</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A313" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B313" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C313" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D313" s="22" t="str">
+        <f t="shared" si="7"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.PROJ_CREATE_DTM IS 'The date/time the project was created';</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A314" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B314" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C314" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D314" s="22" t="str">
+        <f t="shared" si="7"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.PROJ_UPDATE_DTM IS 'The date/time the project was last updated';</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A315" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B315" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C315" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D315" s="22" t="str">
+        <f t="shared" si="7"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.PROJ_VISIBILITY IS 'The visibility for the project (public, internal, private)';</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A316" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B316" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C316" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D316" s="22" t="str">
+        <f t="shared" si="7"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.PROJ_NAME_SPACE IS 'project name including the namespace prefix';</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A317" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B317" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C317" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D317" s="22" t="str">
+        <f t="shared" si="7"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.PROJ_SOURCE IS 'the source of the project record (e.g. PIFSC GitLab, GitHub, manual entry)';</v>
       </c>
     </row>
     <row r="320" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -8375,47 +8726,920 @@
       <c r="C320" s="19"/>
       <c r="D320" s="22"/>
     </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A321" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B321" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C321" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D321" s="22" t="str">
+        <f t="shared" ref="D321:D345" si="8">CONCATENATE("COMMENT ON COLUMN ",A321, ".", B321, " IS '", SUBSTITUTE(C321, "'", "''"), "';")</f>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_ID IS 'Primary key for the PRI_PROJ table';</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A322" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B322" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C322" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D322" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_NAME IS 'Name of the project';</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A323" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B323" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C323" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D323" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_ID IS 'Primary key for the PRI_PROJ_RES table';</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A324" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B324" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C324" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D324" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_NAME IS 'The name of the project resource';</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A325" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B325" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C325" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D325" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_MAX_VERS_NUM IS 'The parsed version number for the maximum installed version of the given resource';</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A326" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B326" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="C326" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="D326" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.CURR_VERS_COUNT IS 'The number of projects that have implemented the given resource that are the same as the current version';</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A327" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B327" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="C327" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="D327" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.OLD_VERS_COUNT IS 'The number of projects that have implemented the given resource that are not the same as the current version';</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A328" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B328" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="C328" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="D328" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.TOTAL_IMPL_PROJ IS 'The total number of projects that have implemented the given resource';</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A329" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B329" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="C329" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="D329" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.ASSOC_PROJ_CD_LIST IS 'A comma-delimited list of projects and associated highest version number that have implemented the given resource.  If the current version implemented is the same as the current version of the resource the project name is preceded by a "*CV" prefix to indicate it is the current version and if not the "*UA" prefix is used to indicate there is an update available';</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A330" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B330" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="C330" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="D330" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.ASSOC_PROJ_BR_LIST IS 'A web line-break-delimited (&lt;BR&gt;) list of projects and associated highest version number that have implemented the given resource.  If the current version implemented is the same as the current version of the resource the project name is preceded by a "*CV" prefix to indicate it is the current version and if not the "*UA" prefix is used to indicate there is an update available';</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A331" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B331" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="C331" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="D331" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.ASSOC_PROJ_LINK_BR_LIST IS 'A web line-break-delimited (&lt;BR&gt;) list of projects and associated highest version number in a formatted hyperlink with a relative path to the given Resource Inventory App project that has implemented the given resource.  If the current version implemented is the same as the current version of the resource the project name is preceded by a "*CV" prefix to indicate it is the current version and if not the "*UA" prefix is used to indicate there is an update available';</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A332" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B332" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C332" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="D332" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_CATEGORY IS 'The resource category (free form text) - examples values include Development Tool, Data Management Tool, Centralized Database Applications';</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A333" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B333" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C333" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D333" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_TAG_CONV IS 'Tag Naming convention used to identify the given project resource''s version.  The suffix is required to be a series of period-delimited numbers (e.g. for a naming convention of db_module_packager_v the tag value of db_module_packager_v1.13.4 is valid)';</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A334" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B334" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C334" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="D334" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_COLOR_CODE IS 'The color code for the project resource';</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A335" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B335" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C335" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D335" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_URL IS 'The URL for the project resource (this is blank when the repository URL is the same as the resource URL)';</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A336" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B336" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C336" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="D336" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_SCOPE_ID IS 'Foreign key reference to the resource scope';</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A337" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B337" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C337" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="D337" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_SCOPE_CODE IS 'Code for the given Resource Scope';</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A338" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B338" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="C338" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D338" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_SCOPE_NAME IS 'Name of the given Resource Scope';</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A339" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B339" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C339" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D339" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_SCOPE_DESC IS 'Description for the given Resource Scope';</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A340" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B340" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C340" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D340" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_TYPE_ID IS 'Foreign key reference to the resource type';</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A341" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B341" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C341" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="D341" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_TYPE_CODE IS 'Code for the given Resource Type';</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A342" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B342" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C342" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="D342" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_TYPE_NAME IS 'Name of the given Resource Type';</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A343" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B343" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="C343" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="D343" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_TYPE_DESC IS 'Description for the given Resource Type';</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A344" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B344" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="C344" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="D344" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_DESC IS 'The description for the project resource';</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A345" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B345" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="C345" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="D345" s="22" t="str">
+        <f t="shared" si="8"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_DEMO_URL IS 'The live demonstration URL for the project resource';</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A350" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B350" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C350" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D350" s="22" t="str">
+        <f t="shared" ref="D350:D385" si="9">CONCATENATE("COMMENT ON COLUMN ",A350, ".", B350, " IS '", SUBSTITUTE(C350, "'", "''"), "';")</f>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_ID IS 'Primary key for the PRI_PROJ table';</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A351" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B351" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C351" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D351" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_NAME IS 'Name of the project';</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A352" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B352" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C352" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D352" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_ID IS 'Primary key for the PRI_PROJ_RES table';</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A353" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B353" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C353" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D353" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_NAME IS 'The name of the project resource';</v>
+      </c>
+    </row>
     <row r="354" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A354" s="19"/>
-      <c r="B354" s="19"/>
-      <c r="C354" s="19"/>
-      <c r="D354" s="22"/>
+      <c r="A354" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B354" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C354" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D354" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_MAX_VERS_NUM IS 'The parsed version number for the maximum installed version of the given resource';</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A355" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B355" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="C355" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="D355" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.CURR_VERS_COUNT IS 'The number of projects that have implemented the given resource that are the same as the current version';</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A356" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B356" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="C356" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="D356" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.OLD_VERS_COUNT IS 'The number of projects that have implemented the given resource that are not the same as the current version';</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A357" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B357" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="C357" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="D357" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.TOTAL_IMPL_PROJ IS 'The total number of projects that have implemented the given resource';</v>
+      </c>
     </row>
     <row r="358" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A358" s="19"/>
-      <c r="B358" s="19"/>
-      <c r="C358" s="19"/>
-      <c r="D358" s="22"/>
+      <c r="A358" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B358" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="C358" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="D358" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.ASSOC_PROJ_CD_LIST IS 'A comma-delimited list of projects and associated highest version number that have implemented the given resource.  If the current version implemented is the same as the current version of the resource the project name is preceded by a "*CV" prefix to indicate it is the current version and if not the "*UA" prefix is used to indicate there is an update available';</v>
+      </c>
     </row>
     <row r="359" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A359" s="19"/>
-      <c r="B359" s="19"/>
-      <c r="C359" s="19"/>
-      <c r="D359" s="22"/>
+      <c r="A359" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B359" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="C359" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="D359" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.ASSOC_PROJ_BR_LIST IS 'A web line-break-delimited (&lt;BR&gt;) list of projects and associated highest version number that have implemented the given resource.  If the current version implemented is the same as the current version of the resource the project name is preceded by a "*CV" prefix to indicate it is the current version and if not the "*UA" prefix is used to indicate there is an update available';</v>
+      </c>
     </row>
     <row r="360" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A360" s="19"/>
-      <c r="B360" s="19"/>
-      <c r="C360" s="19"/>
-      <c r="D360" s="22"/>
+      <c r="A360" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B360" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="C360" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="D360" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.ASSOC_PROJ_LINK_BR_LIST IS 'A web line-break-delimited (&lt;BR&gt;) list of projects and associated highest version number in a formatted hyperlink with a relative path to the given Resource Inventory App project that has implemented the given resource.  If the current version implemented is the same as the current version of the resource the project name is preceded by a "*CV" prefix to indicate it is the current version and if not the "*UA" prefix is used to indicate there is an update available';</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A361" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B361" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C361" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D361" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.VC_PROJ_ID IS 'Unique numeric ID of the project in the given version control system';</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A362" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B362" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C362" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D362" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_DESC IS 'Description of the project';</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A363" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B363" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C363" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D363" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.SSH_URL IS 'SSH URL for the project';</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A364" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B364" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C364" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D364" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.HTTP_URL IS 'HTTP URL for the project';</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A365" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B365" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C365" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D365" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.README_URL IS 'Readme URL for the project';</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A366" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B366" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C366" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D366" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.AVATAR_URL IS 'Avatar URL for the project';</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A367" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B367" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C367" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D367" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_CREATE_DTM IS 'The date/time the project was created';</v>
+      </c>
+    </row>
+    <row r="368" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A368" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B368" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C368" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D368" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_UPDATE_DTM IS 'The date/time the project was last updated';</v>
+      </c>
+    </row>
+    <row r="369" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A369" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B369" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C369" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D369" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_VISIBILITY IS 'The visibility for the project (public, internal, private)';</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A370" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B370" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C370" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D370" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_NAME_SPACE IS 'project name including the namespace prefix';</v>
+      </c>
+    </row>
+    <row r="371" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A371" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B371" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C371" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D371" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_SOURCE IS 'the source of the project record (e.g. PIFSC GitLab, GitHub, manual entry)';</v>
+      </c>
+    </row>
+    <row r="372" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A372" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B372" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C372" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="D372" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_CATEGORY IS 'The resource category (free form text) - examples values include Development Tool, Data Management Tool, Centralized Database Applications';</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A373" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B373" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C373" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D373" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_TAG_CONV IS 'Tag Naming convention used to identify the given project resource''s version.  The suffix is required to be a series of period-delimited numbers (e.g. for a naming convention of db_module_packager_v the tag value of db_module_packager_v1.13.4 is valid)';</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A374" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B374" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C374" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="D374" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_COLOR_CODE IS 'The color code for the project resource';</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A375" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B375" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C375" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D375" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_URL IS 'The URL for the project resource (this is blank when the repository URL is the same as the resource URL)';</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A376" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B376" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C376" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="D376" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_SCOPE_ID IS 'Foreign key reference to the resource scope';</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A377" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B377" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C377" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="D377" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_SCOPE_CODE IS 'Code for the given Resource Scope';</v>
+      </c>
     </row>
     <row r="378" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A378" s="19"/>
-      <c r="B378" s="19"/>
-      <c r="C378" s="19"/>
-      <c r="D378" s="22"/>
+      <c r="A378" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B378" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="C378" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D378" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_SCOPE_NAME IS 'Name of the given Resource Scope';</v>
+      </c>
     </row>
     <row r="379" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A379" s="19"/>
-      <c r="B379" s="19"/>
-      <c r="C379" s="19"/>
-      <c r="D379" s="22"/>
+      <c r="A379" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B379" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C379" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D379" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_SCOPE_DESC IS 'Description for the given Resource Scope';</v>
+      </c>
     </row>
     <row r="380" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A380" s="19"/>
-      <c r="B380" s="19"/>
-      <c r="C380" s="19"/>
-      <c r="D380" s="22"/>
+      <c r="A380" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B380" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C380" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D380" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_TYPE_ID IS 'Foreign key reference to the resource type';</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A381" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B381" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C381" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="D381" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_TYPE_CODE IS 'Code for the given Resource Type';</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A382" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B382" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C382" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="D382" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_TYPE_NAME IS 'Name of the given Resource Type';</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A383" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B383" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="C383" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="D383" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_TYPE_DESC IS 'Description for the given Resource Type';</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A384" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B384" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="C384" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="D384" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_DESC IS 'The description for the project resource';</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A385" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B385" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="C385" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="D385" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_DEMO_URL IS 'The live demonstration URL for the project resource';</v>
+      </c>
     </row>
     <row r="399" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A399" s="19"/>
@@ -11334,10 +12558,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C207"/>
+  <dimension ref="A1:C246"/>
   <sheetViews>
-    <sheetView topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="C181" sqref="C181:C207"/>
+    <sheetView topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="C222" sqref="C222:C246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13604,6 +14828,438 @@
       <c r="C207" s="18" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve">PRI_PROJ_V.RES_TYPE_DESC RES_RES_TYPE_DESC, </v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>177</v>
+      </c>
+      <c r="B211" t="s">
+        <v>72</v>
+      </c>
+      <c r="C211" s="18" t="str">
+        <f t="shared" ref="C211:C246" si="8">CONCATENATE(A211, ".", B211, ", ")</f>
+        <v xml:space="preserve">PRI_RES_PROJ_TAG_MAX_SUM_V.PROJ_ID, </v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B212" t="s">
+        <v>74</v>
+      </c>
+      <c r="C212" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_RES_PROJ_TAG_MAX_SUM_V.PROJ_NAME, </v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B213" t="s">
+        <v>120</v>
+      </c>
+      <c r="C213" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_RES_PROJ_TAG_MAX_SUM_V.RES_ID, </v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B214" t="s">
+        <v>123</v>
+      </c>
+      <c r="C214" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_RES_PROJ_TAG_MAX_SUM_V.RES_NAME, </v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B215" t="s">
+        <v>172</v>
+      </c>
+      <c r="C215" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_RES_PROJ_TAG_MAX_SUM_V.RES_MAX_VERS_NUM, </v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B216" t="s">
+        <v>173</v>
+      </c>
+      <c r="C216" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_RES_PROJ_TAG_MAX_SUM_V.CURR_VERS_COUNT, </v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B217" t="s">
+        <v>174</v>
+      </c>
+      <c r="C217" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_RES_PROJ_TAG_MAX_SUM_V.OLD_VERS_COUNT, </v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B218" t="s">
+        <v>175</v>
+      </c>
+      <c r="C218" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_RES_PROJ_TAG_MAX_SUM_V.TOTAL_IMPL_PROJ, </v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B219" t="s">
+        <v>176</v>
+      </c>
+      <c r="C219" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_RES_PROJ_TAG_MAX_SUM_V.ASSOC_PROJ_CD_LIST, </v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B220" t="s">
+        <v>262</v>
+      </c>
+      <c r="C220" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_RES_PROJ_TAG_MAX_SUM_V.ASSOC_PROJ_BR_LIST, </v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B221" t="s">
+        <v>263</v>
+      </c>
+      <c r="C221" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_RES_PROJ_TAG_MAX_SUM_V.ASSOC_PROJ_LINK_BR_LIST, </v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B222" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C222" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.VC_PROJ_ID, </v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B223" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C223" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.PROJ_DESC, </v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B224" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C224" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.SSH_URL, </v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B225" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C225" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.HTTP_URL, </v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B226" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C226" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.README_URL, </v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B227" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C227" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.AVATAR_URL, </v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B228" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C228" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.PROJ_CREATE_DTM, </v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B229" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C229" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.PROJ_UPDATE_DTM, </v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B230" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C230" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.PROJ_VISIBILITY, </v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B231" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C231" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.PROJ_NAME_SPACE, </v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B232" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C232" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.PROJ_SOURCE, </v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B233" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C233" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_CATEGORY, </v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B234" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C234" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_TAG_CONV, </v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B235" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C235" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_COLOR_CODE, </v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B236" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C236" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_URL, </v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B237" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C237" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_SCOPE_ID, </v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B238" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C238" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_SCOPE_CODE, </v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B239" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C239" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_SCOPE_NAME, </v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B240" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C240" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_SCOPE_DESC, </v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B241" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C241" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_TYPE_ID, </v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B242" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C242" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_TYPE_CODE, </v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B243" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="C243" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_TYPE_NAME, </v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B244" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C244" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_TYPE_DESC, </v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B245" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="C245" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_DESC, </v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B246" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="C246" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_DEMO_URL, </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented additional fields in the GIM
Updated the PRI database to add users, and data sources as tables.  Added new project auditing view fields and new views to utilize the new tables
</commit_message>
<xml_diff>
--- a/docs/DB_DDL_helper_template.xlsx
+++ b/docs/DB_DDL_helper_template.xlsx
@@ -737,7 +737,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="347">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -1554,6 +1554,232 @@
   </si>
   <si>
     <t>The live demonstration URL for the project resource</t>
+  </si>
+  <si>
+    <t>VC_OWNER_ID</t>
+  </si>
+  <si>
+    <t>VC_CREATOR_ID</t>
+  </si>
+  <si>
+    <t>VC_WEB_URL</t>
+  </si>
+  <si>
+    <t>VC_OPEN_ISSUES_COUNT</t>
+  </si>
+  <si>
+    <t>VC_COMMIT_COUNT</t>
+  </si>
+  <si>
+    <t>VC_STORAGE_SIZE</t>
+  </si>
+  <si>
+    <t>VC_REPO_SIZE</t>
+  </si>
+  <si>
+    <t>Unique numeric User ID of the project's owner in the given version control system</t>
+  </si>
+  <si>
+    <t>Unique numeric User ID of the project's creator in the given version control system</t>
+  </si>
+  <si>
+    <t>The web URL of the project in the given version control system</t>
+  </si>
+  <si>
+    <t>The number of open issues for the project in the given version control system</t>
+  </si>
+  <si>
+    <t>The total number of commits for the project in the given version control system</t>
+  </si>
+  <si>
+    <t>The total storage size for the project in the given version control system</t>
+  </si>
+  <si>
+    <t>The total repository size for the project in the given version control system</t>
+  </si>
+  <si>
+    <t>PRI_VC_USERS</t>
+  </si>
+  <si>
+    <t>USER_ID</t>
+  </si>
+  <si>
+    <t>SOURCE_ID</t>
+  </si>
+  <si>
+    <t>Data Sources</t>
+  </si>
+  <si>
+    <t>SOURCE</t>
+  </si>
+  <si>
+    <t>PRI_DATA_SOURCES</t>
+  </si>
+  <si>
+    <t>PIFSC Resource Inventory Data Sources
+This table store the data sources for the information in the PIFSC Resource Inventory Database</t>
+  </si>
+  <si>
+    <t>VC_USER_ID</t>
+  </si>
+  <si>
+    <t>USERNAME</t>
+  </si>
+  <si>
+    <t>USER_NAME</t>
+  </si>
+  <si>
+    <t>USER_EMAIL</t>
+  </si>
+  <si>
+    <t>WEB_URL</t>
+  </si>
+  <si>
+    <t>DATA_SOURCE_ID</t>
+  </si>
+  <si>
+    <t>DATA_SOURCE_CODE</t>
+  </si>
+  <si>
+    <t>DATA_SOURCE_NAME</t>
+  </si>
+  <si>
+    <t>DATA_SOURCE_DESC</t>
+  </si>
+  <si>
+    <t>Primary key for the Data Sources table</t>
+  </si>
+  <si>
+    <t>Code for the given Data Source</t>
+  </si>
+  <si>
+    <t>Name of the given Data Source</t>
+  </si>
+  <si>
+    <t>Description for the given Data Source</t>
+  </si>
+  <si>
+    <t>Primary key for the PRI_VC_USERS table</t>
+  </si>
+  <si>
+    <t>Unique User ID for user within the version control system</t>
+  </si>
+  <si>
+    <t>Login username for the user account in the version control system</t>
+  </si>
+  <si>
+    <t>Name of the user account in the version control system</t>
+  </si>
+  <si>
+    <t>Email for the user account in the version control system</t>
+  </si>
+  <si>
+    <t>Avatar URL for the user account in the version control system</t>
+  </si>
+  <si>
+    <t>Web URL for the user account in the version control system</t>
+  </si>
+  <si>
+    <t>The date on which this user was created in the database</t>
+  </si>
+  <si>
+    <t>The Oracle username of the person creating the user in the database</t>
+  </si>
+  <si>
+    <t>The last date on which any of the data in the user was changed</t>
+  </si>
+  <si>
+    <t>The Oracle username of the person making the most recent change to this user</t>
+  </si>
+  <si>
+    <t>PRI_CV_USERS_V</t>
+  </si>
+  <si>
+    <t>PRI_CV_USERS</t>
+  </si>
+  <si>
+    <t>OWNER_USER_ID</t>
+  </si>
+  <si>
+    <t>OWNER_USERNAME</t>
+  </si>
+  <si>
+    <t>OWNER_USER_NAME</t>
+  </si>
+  <si>
+    <t>OWNER_USER_EMAIL</t>
+  </si>
+  <si>
+    <t>OWNER_AVATAR_URL</t>
+  </si>
+  <si>
+    <t>OWNER_WEB_URL</t>
+  </si>
+  <si>
+    <t>CREATOR_USER_ID</t>
+  </si>
+  <si>
+    <t>CREATOR_USERNAME</t>
+  </si>
+  <si>
+    <t>CREATOR_USER_NAME</t>
+  </si>
+  <si>
+    <t>CREATOR_USER_EMAIL</t>
+  </si>
+  <si>
+    <t>CREATOR_AVATAR_URL</t>
+  </si>
+  <si>
+    <t>CREATOR_WEB_URL</t>
+  </si>
+  <si>
+    <t>The date the project record was created in the database</t>
+  </si>
+  <si>
+    <t>The Oracle username of the person that created the project record in the database</t>
+  </si>
+  <si>
+    <t>The last date on which any of the data in the project record was changed</t>
+  </si>
+  <si>
+    <t>The Oracle username of the person making the most recent change to the project record</t>
+  </si>
+  <si>
+    <t>Login username for the project owner's user account in the version control system</t>
+  </si>
+  <si>
+    <t>Name of the project owner's user account in the version control system</t>
+  </si>
+  <si>
+    <t>Email for the project owner's user account in the version control system</t>
+  </si>
+  <si>
+    <t>Avatar URL for the project owner's user account in the version control system</t>
+  </si>
+  <si>
+    <t>Web URL for the project owner's user account in the version control system</t>
+  </si>
+  <si>
+    <t>The Project Owner's User ID for the version control system</t>
+  </si>
+  <si>
+    <t>The Project Creator's User ID for the version control system</t>
+  </si>
+  <si>
+    <t>Login username for the project creator's user account in the version control system</t>
+  </si>
+  <si>
+    <t>Name of the project creator's user account in the version control system</t>
+  </si>
+  <si>
+    <t>Email for the project creator's user account in the version control system</t>
+  </si>
+  <si>
+    <t>Avatar URL for the project creator's user account in the version control system</t>
+  </si>
+  <si>
+    <t>Web URL for the project creator's user account in the version control system</t>
   </si>
 </sst>
 </file>
@@ -2004,11 +2230,11 @@
   <dimension ref="A1:AA32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="8655" ySplit="900" topLeftCell="T1" activePane="bottomRight"/>
+      <pane xSplit="8655" ySplit="900" activePane="bottomRight"/>
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="T8" sqref="T8"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3560,11 +3786,11 @@
         <v>COMMENT ON TABLE PRI_RES_TYPES IS '';</v>
       </c>
       <c r="Q9" s="22" t="str">
-        <f t="shared" ref="Q9" si="39">CONCATENATE("COMMENT ON COLUMN ", A9, ".", C9, " IS 'Primary Key for the ", A9, " table';")</f>
+        <f t="shared" ref="Q9:Q10" si="39">CONCATENATE("COMMENT ON COLUMN ", A9, ".", C9, " IS 'Primary Key for the ", A9, " table';")</f>
         <v>COMMENT ON COLUMN PRI_RES_TYPES.RES_TYPE_ID IS 'Primary Key for the PRI_RES_TYPES table';</v>
       </c>
       <c r="R9" s="23" t="str">
-        <f t="shared" ref="R9" si="40">CONCATENATE("create or replace TRIGGER 
+        <f t="shared" ref="R9:R10" si="40">CONCATENATE("create or replace TRIGGER 
 ",A9, "_AUTO_BRI 
 before insert on ",A9,"
 for each row
@@ -3584,7 +3810,7 @@
 </v>
       </c>
       <c r="S9" s="23" t="str">
-        <f t="shared" ref="S9" si="41">CONCATENATE("create or replace TRIGGER ",A9, "_AUTO_BRI
+        <f t="shared" ref="S9:S10" si="41">CONCATENATE("create or replace TRIGGER ",A9, "_AUTO_BRI
 before insert on ", A9, "
 for each row
 begin
@@ -3745,12 +3971,16 @@
       </c>
     </row>
     <row r="10" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="19" t="s">
+        <v>286</v>
+      </c>
       <c r="B10" s="16" t="str">
         <f t="shared" si="25"/>
         <v>Yes</v>
       </c>
-      <c r="C10" s="19"/>
+      <c r="C10" s="19" t="s">
+        <v>287</v>
+      </c>
       <c r="D10" s="16" t="str">
         <f t="shared" si="26"/>
         <v>Yes</v>
@@ -3758,61 +3988,408 @@
       <c r="E10" s="19"/>
       <c r="F10" s="16" t="str">
         <f t="shared" si="15"/>
-        <v>_SEQ</v>
-      </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22"/>
-      <c r="V10" s="19"/>
-      <c r="W10" s="19"/>
-      <c r="X10" s="28"/>
-      <c r="Y10" s="28"/>
+        <v>PRI_VC_USERS_SEQ</v>
+      </c>
+      <c r="G10" s="22" t="str">
+        <f t="shared" ref="G10:G11" si="46">CONCATENATE("CREATE SEQUENCE ",F10," INCREMENT BY 1 START WITH 1;")</f>
+        <v>CREATE SEQUENCE PRI_VC_USERS_SEQ INCREMENT BY 1 START WITH 1;</v>
+      </c>
+      <c r="H10" s="22" t="str">
+        <f t="shared" ref="H10:H11" si="47">CONCATENATE("ALTER TABLE ", A10, " ADD (CREATE_DATE DATE );")</f>
+        <v>ALTER TABLE PRI_VC_USERS ADD (CREATE_DATE DATE );</v>
+      </c>
+      <c r="I10" s="22" t="str">
+        <f t="shared" ref="I10:I11" si="48">CONCATENATE("ALTER TABLE ",A10, " ADD (CREATED_BY VARCHAR2(30) );")</f>
+        <v>ALTER TABLE PRI_VC_USERS ADD (CREATED_BY VARCHAR2(30) );</v>
+      </c>
+      <c r="J10" s="22" t="str">
+        <f t="shared" ref="J10:J11" si="49">CONCATENATE("ALTER TABLE ",A10, " ADD (LAST_MOD_DATE DATE );")</f>
+        <v>ALTER TABLE PRI_VC_USERS ADD (LAST_MOD_DATE DATE );</v>
+      </c>
+      <c r="K10" s="22" t="str">
+        <f t="shared" ref="K10:K11" si="50">CONCATENATE("ALTER TABLE ", A10, " ADD (LAST_MOD_BY VARCHAR2(30) );")</f>
+        <v>ALTER TABLE PRI_VC_USERS ADD (LAST_MOD_BY VARCHAR2(30) );</v>
+      </c>
+      <c r="L10" s="22" t="str">
+        <f t="shared" ref="L10:L11" si="51">CONCATENATE("COMMENT ON COLUMN ",A10, ".CREATE_DATE IS 'The date on which this record was created in the database';")</f>
+        <v>COMMENT ON COLUMN PRI_VC_USERS.CREATE_DATE IS 'The date on which this record was created in the database';</v>
+      </c>
+      <c r="M10" s="22" t="str">
+        <f t="shared" ref="M10:M11" si="52">CONCATENATE("COMMENT ON COLUMN ",A10,".CREATED_BY IS 'The Oracle username of the person creating this record in the database';")</f>
+        <v>COMMENT ON COLUMN PRI_VC_USERS.CREATED_BY IS 'The Oracle username of the person creating this record in the database';</v>
+      </c>
+      <c r="N10" s="22" t="str">
+        <f t="shared" ref="N10:N11" si="53">CONCATENATE("COMMENT ON COLUMN ", A10, ".LAST_MOD_DATE IS 'The last date on which any of the data in this record was changed';")</f>
+        <v>COMMENT ON COLUMN PRI_VC_USERS.LAST_MOD_DATE IS 'The last date on which any of the data in this record was changed';</v>
+      </c>
+      <c r="O10" s="22" t="str">
+        <f t="shared" ref="O10:O11" si="54">CONCATENATE("COMMENT ON COLUMN ", A10, ".LAST_MOD_BY IS 'The Oracle username of the person making the most recent change to this record';")</f>
+        <v>COMMENT ON COLUMN PRI_VC_USERS.LAST_MOD_BY IS 'The Oracle username of the person making the most recent change to this record';</v>
+      </c>
+      <c r="P10" s="23" t="str">
+        <f t="shared" ref="P10:P11" si="55">CONCATENATE("COMMENT ON TABLE ", A10, " IS '", SUBSTITUTE(E10, "'", "''"), "';")</f>
+        <v>COMMENT ON TABLE PRI_VC_USERS IS '';</v>
+      </c>
+      <c r="Q10" s="22" t="str">
+        <f t="shared" ref="Q10:Q11" si="56">CONCATENATE("COMMENT ON COLUMN ", A10, ".", C10, " IS 'Primary Key for the ", A10, " table';")</f>
+        <v>COMMENT ON COLUMN PRI_VC_USERS.USER_ID IS 'Primary Key for the PRI_VC_USERS table';</v>
+      </c>
+      <c r="R10" s="23" t="str">
+        <f t="shared" ref="R10:R11" si="57">CONCATENATE("create or replace TRIGGER 
+",A10, "_AUTO_BRI 
+before insert on ",A10,"
+for each row
+begin
+  select ",A10,"_SEQ.nextval into :new.",C10," from dual;
+end;
+/
+")</f>
+        <v xml:space="preserve">create or replace TRIGGER 
+PRI_VC_USERS_AUTO_BRI 
+before insert on PRI_VC_USERS
+for each row
+begin
+  select PRI_VC_USERS_SEQ.nextval into :new.USER_ID from dual;
+end;
+/
+</v>
+      </c>
+      <c r="S10" s="23" t="str">
+        <f t="shared" ref="S10:S11" si="58">CONCATENATE("create or replace TRIGGER ",A10, "_AUTO_BRI
+before insert on ", A10, "
+for each row
+begin
+  select ", A10, "_SEQ.nextval into :new.", C10, " from dual;
+  :NEW.CREATE_DATE := SYSDATE;
+  :NEW.CREATED_BY := nvl(v('APP_USER'),user);
+end;
+/
+")</f>
+        <v xml:space="preserve">create or replace TRIGGER PRI_VC_USERS_AUTO_BRI
+before insert on PRI_VC_USERS
+for each row
+begin
+  select PRI_VC_USERS_SEQ.nextval into :new.USER_ID from dual;
+  :NEW.CREATE_DATE := SYSDATE;
+  :NEW.CREATED_BY := nvl(v('APP_USER'),user);
+end;
+/
+</v>
+      </c>
+      <c r="T10" s="23" t="str">
+        <f t="shared" ref="T10:T11" si="59">CONCATENATE("CREATE OR REPLACE TRIGGER ", A10, "_AUTO_BRU BEFORE
+  UPDATE
+    ON ", A10, " FOR EACH ROW 
+    BEGIN 
+      :NEW.LAST_MOD_DATE := SYSDATE;
+      :NEW.LAST_MOD_BY := nvl(v('APP_USER'),user);
+END;
+/
+")</f>
+        <v xml:space="preserve">CREATE OR REPLACE TRIGGER PRI_VC_USERS_AUTO_BRU BEFORE
+  UPDATE
+    ON PRI_VC_USERS FOR EACH ROW 
+    BEGIN 
+      :NEW.LAST_MOD_DATE := SYSDATE;
+      :NEW.LAST_MOD_BY := nvl(v('APP_USER'),user);
+END;
+/
+</v>
+      </c>
+      <c r="U10" s="18"/>
+      <c r="V10" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="W10" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="X10" s="27" t="str">
+        <f t="shared" ref="X10:X11" si="60">CONCATENATE("CREATE TABLE ", A10, " 
+(
+  ", C10, " NUMBER NOT NULL 
+, ", W10, "_CODE VARCHAR2(50) 
+, ", W10, "_NAME VARCHAR2(200) NOT NULL 
+, ", W10, "_DESC VARCHAR2(500) 
+, CONSTRAINT ", A10, "_PK PRIMARY KEY 
+  (
+    ", C10, " 
+  )
+  ENABLE 
+);
+COMMENT ON COLUMN ", A10, ".", C10, " IS 'Primary key for the ", V10, " table';
+COMMENT ON COLUMN ", A10, ".", W10, "_CODE IS 'Code for the given ", V10, "';
+COMMENT ON COLUMN ", A10, ".", W10, "_NAME IS 'Name of the given ", V10, "';
+COMMENT ON COLUMN ", A10, ".", W10, "_DESC IS 'Description for the given ", V10, "';
+COMMENT ON TABLE ", A10, " IS '", "Reference Table for storing ", V10, " information';
+ALTER TABLE ", A10, " ADD CONSTRAINT ", A10, "_U1 UNIQUE 
+(
+  ", W10, "_CODE 
+)
+ENABLE;
+ALTER TABLE ", A10, " ADD CONSTRAINT ", A10, "_U2 UNIQUE 
+(
+  ", W10, "_NAME 
+)
+ENABLE;
+")</f>
+        <v xml:space="preserve">CREATE TABLE PRI_VC_USERS 
+(
+  USER_ID NUMBER NOT NULL 
+, TYPE_CODE VARCHAR2(50) 
+, TYPE_NAME VARCHAR2(200) NOT NULL 
+, TYPE_DESC VARCHAR2(500) 
+, CONSTRAINT PRI_VC_USERS_PK PRIMARY KEY 
+  (
+    USER_ID 
+  )
+  ENABLE 
+);
+COMMENT ON COLUMN PRI_VC_USERS.USER_ID IS 'Primary key for the Resource Types table';
+COMMENT ON COLUMN PRI_VC_USERS.TYPE_CODE IS 'Code for the given Resource Types';
+COMMENT ON COLUMN PRI_VC_USERS.TYPE_NAME IS 'Name of the given Resource Types';
+COMMENT ON COLUMN PRI_VC_USERS.TYPE_DESC IS 'Description for the given Resource Types';
+COMMENT ON TABLE PRI_VC_USERS IS 'Reference Table for storing Resource Types information';
+ALTER TABLE PRI_VC_USERS ADD CONSTRAINT PRI_VC_USERS_U1 UNIQUE 
+(
+  TYPE_CODE 
+)
+ENABLE;
+ALTER TABLE PRI_VC_USERS ADD CONSTRAINT PRI_VC_USERS_U2 UNIQUE 
+(
+  TYPE_NAME 
+)
+ENABLE;
+</v>
+      </c>
+      <c r="Y10" s="27" t="str">
+        <f>CONCATENATE("insert into ", A10, " (", W10, "_NAME) SELECT distinct [FIELDNAME] from [TABLENAME] where [FIELDNAME] IS NOT NULL AND [FIELDNAME] &lt;&gt; 'NA';")</f>
+        <v>insert into PRI_VC_USERS (TYPE_NAME) SELECT distinct [FIELDNAME] from [TABLENAME] where [FIELDNAME] IS NOT NULL AND [FIELDNAME] &lt;&gt; 'NA';</v>
+      </c>
+      <c r="Z10" s="16" t="str">
+        <f t="shared" ref="Z10:Z11" si="61">CONCATENATE("DROP TRIGGER ""bi_", A10, """;")</f>
+        <v>DROP TRIGGER "bi_PRI_VC_USERS";</v>
+      </c>
+      <c r="AA10" s="28" t="str">
+        <f t="shared" ref="AA10:AA11" si="62">CONCATENATE("--Define the foreign key reference from [TABLENAME] to ", A10, " and associate the reference records appropriately
+--Populate the foreign key reference on [TABLENAME] to the reference table ", A10, "
+UPDATE [TABLENAME] SET TEMP_DATA = ", C10, ", ", C10, " = NULL;
+--modify the existing column
+ALTER TABLE [TABLENAME]  
+MODIFY (", C10, " NUMBER );
+--create the foreign key reference index:
+CREATE INDEX [INDEXNAME] ON [TABLENAME] (", C10, ");
+--create the foreign key constraint:
+ALTER TABLE [TABLENAME]
+ADD CONSTRAINT [FKNAME] FOREIGN KEY
+(
+  ", C10, "
+)
+REFERENCES ", A10, "
+(
+  ", C10, "
+)
+ENABLE;
+--populate the foreign key field with the reference table relationship:
+UPDATE [TABLENAME] SET ", C10, " = (SELECT ", C10, " FROM ", A10, " WHERE ", W10, "_NAME = [TABLENAME].TEMP_DATA);
+")</f>
+        <v xml:space="preserve">--Define the foreign key reference from [TABLENAME] to PRI_VC_USERS and associate the reference records appropriately
+--Populate the foreign key reference on [TABLENAME] to the reference table PRI_VC_USERS
+UPDATE [TABLENAME] SET TEMP_DATA = USER_ID, USER_ID = NULL;
+--modify the existing column
+ALTER TABLE [TABLENAME]  
+MODIFY (USER_ID NUMBER );
+--create the foreign key reference index:
+CREATE INDEX [INDEXNAME] ON [TABLENAME] (USER_ID);
+--create the foreign key constraint:
+ALTER TABLE [TABLENAME]
+ADD CONSTRAINT [FKNAME] FOREIGN KEY
+(
+  USER_ID
+)
+REFERENCES PRI_VC_USERS
+(
+  USER_ID
+)
+ENABLE;
+--populate the foreign key field with the reference table relationship:
+UPDATE [TABLENAME] SET USER_ID = (SELECT USER_ID FROM PRI_VC_USERS WHERE TYPE_NAME = [TABLENAME].TEMP_DATA);
+</v>
+      </c>
     </row>
     <row r="11" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="19" t="s">
+        <v>291</v>
+      </c>
       <c r="B11" s="16" t="str">
         <f t="shared" si="25"/>
         <v>Yes</v>
       </c>
-      <c r="C11" s="19"/>
+      <c r="C11" s="19" t="s">
+        <v>288</v>
+      </c>
       <c r="D11" s="16" t="str">
         <f t="shared" si="26"/>
         <v>Yes</v>
       </c>
-      <c r="E11" s="19"/>
+      <c r="E11" s="20" t="s">
+        <v>292</v>
+      </c>
       <c r="F11" s="16" t="str">
         <f t="shared" si="15"/>
-        <v>_SEQ</v>
-      </c>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
-      <c r="S11" s="22"/>
-      <c r="T11" s="22"/>
-      <c r="V11" s="19"/>
-      <c r="W11" s="19"/>
-      <c r="X11" s="28"/>
-      <c r="Y11" s="28"/>
+        <v>PRI_DATA_SOURCES_SEQ</v>
+      </c>
+      <c r="G11" s="22" t="str">
+        <f t="shared" si="46"/>
+        <v>CREATE SEQUENCE PRI_DATA_SOURCES_SEQ INCREMENT BY 1 START WITH 1;</v>
+      </c>
+      <c r="H11" s="22" t="str">
+        <f t="shared" si="47"/>
+        <v>ALTER TABLE PRI_DATA_SOURCES ADD (CREATE_DATE DATE );</v>
+      </c>
+      <c r="I11" s="22" t="str">
+        <f t="shared" si="48"/>
+        <v>ALTER TABLE PRI_DATA_SOURCES ADD (CREATED_BY VARCHAR2(30) );</v>
+      </c>
+      <c r="J11" s="22" t="str">
+        <f t="shared" si="49"/>
+        <v>ALTER TABLE PRI_DATA_SOURCES ADD (LAST_MOD_DATE DATE );</v>
+      </c>
+      <c r="K11" s="22" t="str">
+        <f t="shared" si="50"/>
+        <v>ALTER TABLE PRI_DATA_SOURCES ADD (LAST_MOD_BY VARCHAR2(30) );</v>
+      </c>
+      <c r="L11" s="22" t="str">
+        <f t="shared" si="51"/>
+        <v>COMMENT ON COLUMN PRI_DATA_SOURCES.CREATE_DATE IS 'The date on which this record was created in the database';</v>
+      </c>
+      <c r="M11" s="22" t="str">
+        <f t="shared" si="52"/>
+        <v>COMMENT ON COLUMN PRI_DATA_SOURCES.CREATED_BY IS 'The Oracle username of the person creating this record in the database';</v>
+      </c>
+      <c r="N11" s="22" t="str">
+        <f t="shared" si="53"/>
+        <v>COMMENT ON COLUMN PRI_DATA_SOURCES.LAST_MOD_DATE IS 'The last date on which any of the data in this record was changed';</v>
+      </c>
+      <c r="O11" s="22" t="str">
+        <f t="shared" si="54"/>
+        <v>COMMENT ON COLUMN PRI_DATA_SOURCES.LAST_MOD_BY IS 'The Oracle username of the person making the most recent change to this record';</v>
+      </c>
+      <c r="P11" s="22" t="str">
+        <f t="shared" si="55"/>
+        <v>COMMENT ON TABLE PRI_DATA_SOURCES IS 'PIFSC Resource Inventory Data Sources
+This table store the data sources for the information in the PIFSC Resource Inventory Database';</v>
+      </c>
+      <c r="Q11" s="22" t="str">
+        <f t="shared" si="56"/>
+        <v>COMMENT ON COLUMN PRI_DATA_SOURCES.SOURCE_ID IS 'Primary Key for the PRI_DATA_SOURCES table';</v>
+      </c>
+      <c r="R11" s="22" t="str">
+        <f t="shared" si="57"/>
+        <v xml:space="preserve">create or replace TRIGGER 
+PRI_DATA_SOURCES_AUTO_BRI 
+before insert on PRI_DATA_SOURCES
+for each row
+begin
+  select PRI_DATA_SOURCES_SEQ.nextval into :new.SOURCE_ID from dual;
+end;
+/
+</v>
+      </c>
+      <c r="S11" s="22" t="str">
+        <f t="shared" si="58"/>
+        <v xml:space="preserve">create or replace TRIGGER PRI_DATA_SOURCES_AUTO_BRI
+before insert on PRI_DATA_SOURCES
+for each row
+begin
+  select PRI_DATA_SOURCES_SEQ.nextval into :new.SOURCE_ID from dual;
+  :NEW.CREATE_DATE := SYSDATE;
+  :NEW.CREATED_BY := nvl(v('APP_USER'),user);
+end;
+/
+</v>
+      </c>
+      <c r="T11" s="22" t="str">
+        <f t="shared" si="59"/>
+        <v xml:space="preserve">CREATE OR REPLACE TRIGGER PRI_DATA_SOURCES_AUTO_BRU BEFORE
+  UPDATE
+    ON PRI_DATA_SOURCES FOR EACH ROW 
+    BEGIN 
+      :NEW.LAST_MOD_DATE := SYSDATE;
+      :NEW.LAST_MOD_BY := nvl(v('APP_USER'),user);
+END;
+/
+</v>
+      </c>
+      <c r="V11" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="W11" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="X11" s="28" t="str">
+        <f t="shared" si="60"/>
+        <v xml:space="preserve">CREATE TABLE PRI_DATA_SOURCES 
+(
+  SOURCE_ID NUMBER NOT NULL 
+, SOURCE_CODE VARCHAR2(50) 
+, SOURCE_NAME VARCHAR2(200) NOT NULL 
+, SOURCE_DESC VARCHAR2(500) 
+, CONSTRAINT PRI_DATA_SOURCES_PK PRIMARY KEY 
+  (
+    SOURCE_ID 
+  )
+  ENABLE 
+);
+COMMENT ON COLUMN PRI_DATA_SOURCES.SOURCE_ID IS 'Primary key for the Data Sources table';
+COMMENT ON COLUMN PRI_DATA_SOURCES.SOURCE_CODE IS 'Code for the given Data Sources';
+COMMENT ON COLUMN PRI_DATA_SOURCES.SOURCE_NAME IS 'Name of the given Data Sources';
+COMMENT ON COLUMN PRI_DATA_SOURCES.SOURCE_DESC IS 'Description for the given Data Sources';
+COMMENT ON TABLE PRI_DATA_SOURCES IS 'Reference Table for storing Data Sources information';
+ALTER TABLE PRI_DATA_SOURCES ADD CONSTRAINT PRI_DATA_SOURCES_U1 UNIQUE 
+(
+  SOURCE_CODE 
+)
+ENABLE;
+ALTER TABLE PRI_DATA_SOURCES ADD CONSTRAINT PRI_DATA_SOURCES_U2 UNIQUE 
+(
+  SOURCE_NAME 
+)
+ENABLE;
+</v>
+      </c>
+      <c r="Y11" s="28" t="str">
+        <f>CONCATENATE("insert into ", A11, " (", W11, "_NAME) SELECT distinct [FIELDNAME] from [TABLENAME] where [FIELDNAME] IS NOT NULL AND [FIELDNAME] &lt;&gt; 'NA';")</f>
+        <v>insert into PRI_DATA_SOURCES (SOURCE_NAME) SELECT distinct [FIELDNAME] from [TABLENAME] where [FIELDNAME] IS NOT NULL AND [FIELDNAME] &lt;&gt; 'NA';</v>
+      </c>
+      <c r="Z11" s="16" t="str">
+        <f t="shared" si="61"/>
+        <v>DROP TRIGGER "bi_PRI_DATA_SOURCES";</v>
+      </c>
+      <c r="AA11" s="28" t="str">
+        <f t="shared" si="62"/>
+        <v xml:space="preserve">--Define the foreign key reference from [TABLENAME] to PRI_DATA_SOURCES and associate the reference records appropriately
+--Populate the foreign key reference on [TABLENAME] to the reference table PRI_DATA_SOURCES
+UPDATE [TABLENAME] SET TEMP_DATA = SOURCE_ID, SOURCE_ID = NULL;
+--modify the existing column
+ALTER TABLE [TABLENAME]  
+MODIFY (SOURCE_ID NUMBER );
+--create the foreign key reference index:
+CREATE INDEX [INDEXNAME] ON [TABLENAME] (SOURCE_ID);
+--create the foreign key constraint:
+ALTER TABLE [TABLENAME]
+ADD CONSTRAINT [FKNAME] FOREIGN KEY
+(
+  SOURCE_ID
+)
+REFERENCES PRI_DATA_SOURCES
+(
+  SOURCE_ID
+)
+ENABLE;
+--populate the foreign key field with the reference table relationship:
+UPDATE [TABLENAME] SET SOURCE_ID = (SELECT SOURCE_ID FROM PRI_DATA_SOURCES WHERE SOURCE_NAME = [TABLENAME].TEMP_DATA);
+</v>
+      </c>
     </row>
     <row r="12" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
@@ -4560,8 +5137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2806"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A334" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D350" sqref="D350:D385"/>
+    <sheetView tabSelected="1" topLeftCell="A404" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D420" sqref="D420:D435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9641,41 +10218,614 @@
         <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_DEMO_URL IS 'The live demonstration URL for the project resource';</v>
       </c>
     </row>
+    <row r="389" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A389" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B389" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="C389" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="D389" s="22" t="str">
+        <f t="shared" ref="D389:D416" si="10">CONCATENATE("COMMENT ON COLUMN ",A389, ".", B389, " IS '", SUBSTITUTE(C389, "'", "''"), "';")</f>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.VC_OWNER_ID IS 'Unique numeric User ID of the project''s owner in the given version control system';</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A390" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B390" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="C390" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="D390" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.VC_CREATOR_ID IS 'Unique numeric User ID of the project''s creator in the given version control system';</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A391" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B391" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="C391" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="D391" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.VC_WEB_URL IS 'The web URL of the project in the given version control system';</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A392" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B392" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="C392" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="D392" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.VC_OPEN_ISSUES_COUNT IS 'The number of open issues for the project in the given version control system';</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A393" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B393" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="C393" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="D393" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.VC_COMMIT_COUNT IS 'The total number of commits for the project in the given version control system';</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A394" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B394" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="C394" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="D394" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.VC_STORAGE_SIZE IS 'The total storage size for the project in the given version control system';</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A395" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B395" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C395" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="D395" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.VC_REPO_SIZE IS 'The total repository size for the project in the given version control system';</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D396" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN . IS '';</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D397" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN . IS '';</v>
+      </c>
+    </row>
+    <row r="398" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D398" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN . IS '';</v>
+      </c>
+    </row>
     <row r="399" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A399" s="19"/>
       <c r="B399" s="19"/>
       <c r="C399" s="19"/>
-      <c r="D399" s="22"/>
+      <c r="D399" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN . IS '';</v>
+      </c>
     </row>
     <row r="400" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A400" s="19"/>
-      <c r="B400" s="19"/>
-      <c r="C400" s="19"/>
-      <c r="D400" s="22"/>
+      <c r="A400" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B400" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="C400" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="D400" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_CV_USERS_V.USER_ID IS 'Primary key for the PRI_VC_USERS table';</v>
+      </c>
     </row>
     <row r="401" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A401" s="19"/>
-      <c r="B401" s="19"/>
-      <c r="C401" s="19"/>
-      <c r="D401" s="22"/>
+      <c r="A401" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B401" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="C401" s="18" t="s">
+        <v>307</v>
+      </c>
+      <c r="D401" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_CV_USERS_V.VC_USER_ID IS 'Unique User ID for user within the version control system';</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A402" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B402" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="C402" s="18" t="s">
+        <v>308</v>
+      </c>
+      <c r="D402" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_CV_USERS_V.USERNAME IS 'Login username for the user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A403" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B403" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="C403" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="D403" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_CV_USERS_V.USER_NAME IS 'Name of the user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A404" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B404" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="C404" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="D404" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_CV_USERS_V.USER_EMAIL IS 'Email for the user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A405" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B405" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C405" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="D405" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_CV_USERS_V.AVATAR_URL IS 'Avatar URL for the user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A406" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B406" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="C406" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="D406" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_CV_USERS_V.WEB_URL IS 'Web URL for the user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A407" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B407" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="C407" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="D407" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_CV_USERS_V.DATA_SOURCE_ID IS 'Primary key for the Data Sources table';</v>
+      </c>
     </row>
     <row r="408" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A408" s="19"/>
-      <c r="B408" s="19"/>
-      <c r="C408" s="19"/>
-      <c r="D408" s="22"/>
+      <c r="A408" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B408" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="C408" s="18" t="s">
+        <v>303</v>
+      </c>
+      <c r="D408" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_CV_USERS_V.DATA_SOURCE_CODE IS 'Code for the given Data Source';</v>
+      </c>
     </row>
     <row r="409" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A409" s="19"/>
-      <c r="B409" s="19"/>
-      <c r="C409" s="19"/>
-      <c r="D409" s="22"/>
+      <c r="A409" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B409" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="C409" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="D409" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_CV_USERS_V.DATA_SOURCE_NAME IS 'Name of the given Data Source';</v>
+      </c>
     </row>
     <row r="410" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A410" s="19"/>
-      <c r="B410" s="19"/>
-      <c r="C410" s="19"/>
-      <c r="D410" s="22"/>
+      <c r="A410" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B410" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="C410" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="D410" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_CV_USERS_V.DATA_SOURCE_DESC IS 'Description for the given Data Source';</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A411" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B411" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C411" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="D411" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_CV_USERS_V.CREATE_DATE IS 'The date on which this user was created in the database';</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A412" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B412" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C412" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="D412" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_CV_USERS_V.CREATED_BY IS 'The Oracle username of the person creating the user in the database';</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A413" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B413" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C413" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="D413" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_CV_USERS_V.LAST_MOD_DATE IS 'The last date on which any of the data in the user was changed';</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A414" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B414" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C414" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="D414" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN PRI_CV_USERS_V.LAST_MOD_BY IS 'The Oracle username of the person making the most recent change to this user';</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D415" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN . IS '';</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D416" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN . IS '';</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A420" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B420" s="19" t="s">
+        <v>319</v>
+      </c>
+      <c r="C420" s="19" t="s">
+        <v>340</v>
+      </c>
+      <c r="D420" s="22" t="str">
+        <f t="shared" ref="D420:D435" si="11">CONCATENATE("COMMENT ON COLUMN ",A420, ".", B420, " IS '", SUBSTITUTE(C420, "'", "''"), "';")</f>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.OWNER_USER_ID IS 'The Project Owner''s User ID for the version control system';</v>
+      </c>
+    </row>
+    <row r="421" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A421" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B421" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="C421" s="19" t="s">
+        <v>335</v>
+      </c>
+      <c r="D421" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.OWNER_USERNAME IS 'Login username for the project owner''s user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A422" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B422" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="C422" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="D422" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.OWNER_USER_NAME IS 'Name of the project owner''s user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A423" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B423" s="19" t="s">
+        <v>322</v>
+      </c>
+      <c r="C423" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="D423" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.OWNER_USER_EMAIL IS 'Email for the project owner''s user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A424" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B424" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="C424" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="D424" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.OWNER_AVATAR_URL IS 'Avatar URL for the project owner''s user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A425" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B425" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="C425" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="D425" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.OWNER_WEB_URL IS 'Web URL for the project owner''s user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A426" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B426" s="19" t="s">
+        <v>325</v>
+      </c>
+      <c r="C426" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="D426" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.CREATOR_USER_ID IS 'The Project Creator''s User ID for the version control system';</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A427" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B427" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="C427" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="D427" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.CREATOR_USERNAME IS 'Login username for the project creator''s user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A428" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B428" s="19" t="s">
+        <v>327</v>
+      </c>
+      <c r="C428" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="D428" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.CREATOR_USER_NAME IS 'Name of the project creator''s user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A429" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B429" s="19" t="s">
+        <v>328</v>
+      </c>
+      <c r="C429" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="D429" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.CREATOR_USER_EMAIL IS 'Email for the project creator''s user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A430" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B430" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="C430" s="19" t="s">
+        <v>345</v>
+      </c>
+      <c r="D430" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.CREATOR_AVATAR_URL IS 'Avatar URL for the project creator''s user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A431" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B431" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="C431" s="19" t="s">
+        <v>346</v>
+      </c>
+      <c r="D431" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.CREATOR_WEB_URL IS 'Web URL for the project creator''s user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A432" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B432" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C432" s="19" t="s">
+        <v>331</v>
+      </c>
+      <c r="D432" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.CREATE_DATE IS 'The date the project record was created in the database';</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A433" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B433" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C433" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="D433" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.CREATED_BY IS 'The Oracle username of the person that created the project record in the database';</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A434" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B434" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C434" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="D434" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.LAST_MOD_DATE IS 'The last date on which any of the data in the project record was changed';</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A435" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B435" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C435" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="D435" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN PRI_PROJ_RES_TAG_MAX_SUM_ALL_V.LAST_MOD_BY IS 'The Oracle username of the person making the most recent change to the project record';</v>
+      </c>
     </row>
     <row r="436" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A436" s="19"/>
@@ -12558,10 +13708,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C246"/>
+  <dimension ref="A1:C270"/>
   <sheetViews>
-    <sheetView topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="C222" sqref="C222:C246"/>
+    <sheetView topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="C263" sqref="C263:C266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14838,7 +15988,7 @@
         <v>72</v>
       </c>
       <c r="C211" s="18" t="str">
-        <f t="shared" ref="C211:C246" si="8">CONCATENATE(A211, ".", B211, ", ")</f>
+        <f t="shared" ref="C211:C253" si="8">CONCATENATE(A211, ".", B211, ", ")</f>
         <v xml:space="preserve">PRI_RES_PROJ_TAG_MAX_SUM_V.PROJ_ID, </v>
       </c>
     </row>
@@ -15260,6 +16410,270 @@
       <c r="C246" s="18" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">PRI_PROJ_V.RES_DEMO_URL, </v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B247" t="s">
+        <v>272</v>
+      </c>
+      <c r="C247" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.VC_OWNER_ID, </v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B248" t="s">
+        <v>273</v>
+      </c>
+      <c r="C248" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.VC_CREATOR_ID, </v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B249" t="s">
+        <v>274</v>
+      </c>
+      <c r="C249" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.VC_WEB_URL, </v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B250" t="s">
+        <v>275</v>
+      </c>
+      <c r="C250" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.VC_OPEN_ISSUES_COUNT, </v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B251" t="s">
+        <v>276</v>
+      </c>
+      <c r="C251" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.VC_COMMIT_COUNT, </v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B252" t="s">
+        <v>277</v>
+      </c>
+      <c r="C252" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.VC_STORAGE_SIZE, </v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B253" t="s">
+        <v>278</v>
+      </c>
+      <c r="C253" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PRI_PROJ_V.VC_REPO_SIZE, </v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B256" t="s">
+        <v>287</v>
+      </c>
+      <c r="C256" s="18" t="str">
+        <f t="shared" ref="C256:C270" si="9">CONCATENATE(A256, ".", B256, ", ")</f>
+        <v xml:space="preserve">PRI_CV_USERS.USER_ID, </v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B257" t="s">
+        <v>293</v>
+      </c>
+      <c r="C257" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">PRI_CV_USERS.VC_USER_ID, </v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B258" t="s">
+        <v>294</v>
+      </c>
+      <c r="C258" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">PRI_CV_USERS.USERNAME, </v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B259" t="s">
+        <v>295</v>
+      </c>
+      <c r="C259" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">PRI_CV_USERS.USER_NAME, </v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B260" t="s">
+        <v>296</v>
+      </c>
+      <c r="C260" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">PRI_CV_USERS.USER_EMAIL, </v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B261" t="s">
+        <v>79</v>
+      </c>
+      <c r="C261" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">PRI_CV_USERS.AVATAR_URL, </v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B262" t="s">
+        <v>297</v>
+      </c>
+      <c r="C262" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">PRI_CV_USERS.WEB_URL, </v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="B263" t="s">
+        <v>298</v>
+      </c>
+      <c r="C263" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">PRI_DATA_SOURCES.DATA_SOURCE_ID, </v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="B264" t="s">
+        <v>299</v>
+      </c>
+      <c r="C264" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">PRI_DATA_SOURCES.DATA_SOURCE_CODE, </v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="B265" t="s">
+        <v>300</v>
+      </c>
+      <c r="C265" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">PRI_DATA_SOURCES.DATA_SOURCE_NAME, </v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="B266" t="s">
+        <v>301</v>
+      </c>
+      <c r="C266" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">PRI_DATA_SOURCES.DATA_SOURCE_DESC, </v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B267" t="s">
+        <v>98</v>
+      </c>
+      <c r="C267" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">PRI_CV_USERS.CREATE_DATE, </v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B268" t="s">
+        <v>99</v>
+      </c>
+      <c r="C268" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">PRI_CV_USERS.CREATED_BY, </v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B269" t="s">
+        <v>100</v>
+      </c>
+      <c r="C269" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">PRI_CV_USERS.LAST_MOD_DATE, </v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B270" t="s">
+        <v>101</v>
+      </c>
+      <c r="C270" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">PRI_CV_USERS.LAST_MOD_BY, </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the DB to include additional fields in the reporting views
</commit_message>
<xml_diff>
--- a/docs/DB_DDL_helper_template.xlsx
+++ b/docs/DB_DDL_helper_template.xlsx
@@ -737,7 +737,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="356">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -1780,6 +1780,33 @@
   </si>
   <si>
     <t>Web URL for the project creator's user account in the version control system</t>
+  </si>
+  <si>
+    <t>VC_REPO_SIZE_MB</t>
+  </si>
+  <si>
+    <t>PROJ_REFRESH_DATE</t>
+  </si>
+  <si>
+    <t>Primary key for the project's Data Source</t>
+  </si>
+  <si>
+    <t>Code for the given project's Data Source</t>
+  </si>
+  <si>
+    <t>Name of the given project's Data Source</t>
+  </si>
+  <si>
+    <t>Description for the given project's Data Source</t>
+  </si>
+  <si>
+    <t>The total repository size in bytes for the project in the given version control system</t>
+  </si>
+  <si>
+    <t>The total repository size in MB for the project in the given version control system</t>
+  </si>
+  <si>
+    <t>The date of the last time the project information was refreshed in the database</t>
   </si>
 </sst>
 </file>
@@ -3786,11 +3813,11 @@
         <v>COMMENT ON TABLE PRI_RES_TYPES IS '';</v>
       </c>
       <c r="Q9" s="22" t="str">
-        <f t="shared" ref="Q9:Q10" si="39">CONCATENATE("COMMENT ON COLUMN ", A9, ".", C9, " IS 'Primary Key for the ", A9, " table';")</f>
+        <f t="shared" ref="Q9" si="39">CONCATENATE("COMMENT ON COLUMN ", A9, ".", C9, " IS 'Primary Key for the ", A9, " table';")</f>
         <v>COMMENT ON COLUMN PRI_RES_TYPES.RES_TYPE_ID IS 'Primary Key for the PRI_RES_TYPES table';</v>
       </c>
       <c r="R9" s="23" t="str">
-        <f t="shared" ref="R9:R10" si="40">CONCATENATE("create or replace TRIGGER 
+        <f t="shared" ref="R9" si="40">CONCATENATE("create or replace TRIGGER 
 ",A9, "_AUTO_BRI 
 before insert on ",A9,"
 for each row
@@ -3810,7 +3837,7 @@
 </v>
       </c>
       <c r="S9" s="23" t="str">
-        <f t="shared" ref="S9:S10" si="41">CONCATENATE("create or replace TRIGGER ",A9, "_AUTO_BRI
+        <f t="shared" ref="S9" si="41">CONCATENATE("create or replace TRIGGER ",A9, "_AUTO_BRI
 before insert on ", A9, "
 for each row
 begin
@@ -5137,8 +5164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2806"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A404" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D420" sqref="D420:D435"/>
+    <sheetView tabSelected="1" topLeftCell="A438" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C449" sqref="C449"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10840,52 +10867,844 @@
       <c r="D437" s="22"/>
     </row>
     <row r="438" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A438" s="19"/>
-      <c r="B438" s="19"/>
-      <c r="C438" s="19"/>
-      <c r="D438" s="22"/>
+      <c r="A438" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B438" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C438" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D438" s="22" t="str">
+        <f t="shared" ref="D438:D493" si="12">CONCATENATE("COMMENT ON COLUMN ",A438, ".", B438, " IS '", SUBSTITUTE(C438, "'", "''"), "';")</f>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_ID IS 'Primary key for the PRI_PROJ table';</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A439" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B439" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C439" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D439" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.VC_PROJ_ID IS 'Unique numeric ID of the project in the given version control system';</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A440" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B440" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C440" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D440" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_NAME IS 'Name of the project';</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A441" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B441" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C441" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D441" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_DESC IS 'Description of the project';</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A442" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B442" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C442" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D442" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.SSH_URL IS 'SSH URL for the project';</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A443" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B443" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C443" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D443" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.HTTP_URL IS 'HTTP URL for the project';</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A444" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B444" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C444" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D444" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.README_URL IS 'Readme URL for the project';</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A445" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B445" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C445" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D445" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.AVATAR_URL IS 'Avatar URL for the project';</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A446" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B446" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C446" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D446" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_CREATE_DTM IS 'The date/time the project was created';</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A447" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B447" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C447" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D447" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_UPDATE_DTM IS 'The date/time the project was last updated';</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A448" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B448" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C448" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D448" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_VISIBILITY IS 'The visibility for the project (public, internal, private)';</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A449" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B449" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C449" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D449" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_NAME_SPACE IS 'project name including the namespace prefix';</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A450" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B450" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="C450" s="19" t="s">
+        <v>349</v>
+      </c>
+      <c r="D450" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.DATA_SOURCE_ID IS 'Primary key for the project''s Data Source';</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A451" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B451" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="C451" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="D451" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.DATA_SOURCE_CODE IS 'Code for the given project''s Data Source';</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A452" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B452" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="C452" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="D452" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.DATA_SOURCE_NAME IS 'Name of the given project''s Data Source';</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A453" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B453" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="C453" s="19" t="s">
+        <v>352</v>
+      </c>
+      <c r="D453" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.DATA_SOURCE_DESC IS 'Description for the given project''s Data Source';</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A454" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B454" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="C454" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="D454" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.VC_OWNER_ID IS 'Unique numeric User ID of the project''s owner in the given version control system';</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A455" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B455" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="C455" s="19" t="s">
+        <v>340</v>
+      </c>
+      <c r="D455" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.OWNER_USER_ID IS 'The Project Owner''s User ID for the version control system';</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A456" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B456" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="C456" s="19" t="s">
+        <v>335</v>
+      </c>
+      <c r="D456" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.OWNER_USERNAME IS 'Login username for the project owner''s user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A457" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B457" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="C457" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="D457" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.OWNER_USER_NAME IS 'Name of the project owner''s user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A458" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B458" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="C458" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="D458" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.OWNER_USER_EMAIL IS 'Email for the project owner''s user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A459" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B459" s="18" t="s">
+        <v>323</v>
+      </c>
+      <c r="C459" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="D459" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.OWNER_AVATAR_URL IS 'Avatar URL for the project owner''s user account in the version control system';</v>
+      </c>
     </row>
     <row r="460" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A460" s="19"/>
-      <c r="B460" s="19"/>
-      <c r="C460" s="19"/>
-      <c r="D460" s="22"/>
+      <c r="A460" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B460" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="C460" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="D460" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.OWNER_WEB_URL IS 'Web URL for the project owner''s user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A461" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B461" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="C461" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="D461" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.VC_CREATOR_ID IS 'Unique numeric User ID of the project''s creator in the given version control system';</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A462" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B462" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="C462" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="D462" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.CREATOR_USER_ID IS 'The Project Creator''s User ID for the version control system';</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A463" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B463" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="C463" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="D463" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.CREATOR_USERNAME IS 'Login username for the project creator''s user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A464" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B464" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="C464" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="D464" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.CREATOR_USER_NAME IS 'Name of the project creator''s user account in the version control system';</v>
+      </c>
     </row>
     <row r="465" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A465" s="19"/>
-      <c r="B465" s="19"/>
-      <c r="C465" s="19"/>
-      <c r="D465" s="22"/>
+      <c r="A465" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B465" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="C465" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="D465" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.CREATOR_USER_EMAIL IS 'Email for the project creator''s user account in the version control system';</v>
+      </c>
     </row>
     <row r="466" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A466" s="19"/>
-      <c r="B466" s="19"/>
-      <c r="C466" s="19"/>
-      <c r="D466" s="22"/>
+      <c r="A466" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B466" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="C466" s="19" t="s">
+        <v>345</v>
+      </c>
+      <c r="D466" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.CREATOR_AVATAR_URL IS 'Avatar URL for the project creator''s user account in the version control system';</v>
+      </c>
     </row>
     <row r="467" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A467" s="19"/>
-      <c r="B467" s="19"/>
-      <c r="C467" s="19"/>
-      <c r="D467" s="22"/>
+      <c r="A467" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B467" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="C467" s="19" t="s">
+        <v>346</v>
+      </c>
+      <c r="D467" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.CREATOR_WEB_URL IS 'Web URL for the project creator''s user account in the version control system';</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A468" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B468" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="C468" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="D468" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.VC_WEB_URL IS 'The web URL of the project in the given version control system';</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A469" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B469" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="C469" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="D469" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.VC_OPEN_ISSUES_COUNT IS 'The number of open issues for the project in the given version control system';</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A470" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B470" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="C470" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="D470" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.VC_COMMIT_COUNT IS 'The total number of commits for the project in the given version control system';</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A471" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B471" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C471" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="D471" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.VC_REPO_SIZE IS 'The total repository size in bytes for the project in the given version control system';</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A472" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B472" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="C472" s="19" t="s">
+        <v>354</v>
+      </c>
+      <c r="D472" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.VC_REPO_SIZE_MB IS 'The total repository size in MB for the project in the given version control system';</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A473" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B473" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C473" s="19" t="s">
+        <v>331</v>
+      </c>
+      <c r="D473" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.CREATE_DATE IS 'The date the project record was created in the database';</v>
+      </c>
     </row>
     <row r="474" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A474" s="19"/>
-      <c r="B474" s="19"/>
-      <c r="C474" s="19"/>
-      <c r="D474" s="22"/>
+      <c r="A474" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B474" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C474" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="D474" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.CREATED_BY IS 'The Oracle username of the person that created the project record in the database';</v>
+      </c>
     </row>
     <row r="475" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A475" s="19"/>
-      <c r="B475" s="19"/>
-      <c r="C475" s="19"/>
-      <c r="D475" s="22"/>
+      <c r="A475" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B475" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C475" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="D475" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.LAST_MOD_DATE IS 'The last date on which any of the data in the project record was changed';</v>
+      </c>
     </row>
     <row r="476" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A476" s="19"/>
-      <c r="B476" s="19"/>
-      <c r="C476" s="19"/>
-      <c r="D476" s="22"/>
+      <c r="A476" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B476" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C476" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="D476" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.LAST_MOD_BY IS 'The Oracle username of the person making the most recent change to the project record';</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A477" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B477" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="C477" s="19" t="s">
+        <v>355</v>
+      </c>
+      <c r="D477" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.PROJ_REFRESH_DATE IS 'The date of the last time the project information was refreshed in the database';</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A478" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B478" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C478" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D478" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_ID IS 'Primary key for the PRI_PROJ_RES table';</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A479" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B479" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C479" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="D479" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_CATEGORY IS 'The resource category (free form text) - examples values include Development Tool, Data Management Tool, Centralized Database Applications';</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A480" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B480" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C480" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D480" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_TAG_CONV IS 'Tag Naming convention used to identify the given project resource''s version.  The suffix is required to be a series of period-delimited numbers (e.g. for a naming convention of db_module_packager_v the tag value of db_module_packager_v1.13.4 is valid)';</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A481" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B481" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C481" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D481" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_NAME IS 'The name of the project resource';</v>
+      </c>
+    </row>
+    <row r="482" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A482" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B482" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C482" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="D482" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_COLOR_CODE IS 'The color code for the project resource';</v>
+      </c>
+    </row>
+    <row r="483" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A483" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B483" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C483" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D483" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_URL IS 'The URL for the project resource (this is blank when the repository URL is the same as the resource URL)';</v>
+      </c>
+    </row>
+    <row r="484" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A484" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B484" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C484" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="D484" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_SCOPE_ID IS 'Foreign key reference to the resource scope';</v>
+      </c>
+    </row>
+    <row r="485" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A485" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B485" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C485" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="D485" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_SCOPE_CODE IS 'Code for the given Resource Scope';</v>
+      </c>
+    </row>
+    <row r="486" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A486" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B486" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C486" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D486" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_SCOPE_NAME IS 'Name of the given Resource Scope';</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A487" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B487" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C487" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D487" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_SCOPE_DESC IS 'Description for the given Resource Scope';</v>
+      </c>
+    </row>
+    <row r="488" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A488" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B488" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C488" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D488" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_TYPE_ID IS 'Foreign key reference to the resource type';</v>
+      </c>
+    </row>
+    <row r="489" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A489" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B489" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C489" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="D489" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_TYPE_CODE IS 'Code for the given Resource Type';</v>
+      </c>
+    </row>
+    <row r="490" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A490" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B490" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="C490" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="D490" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_TYPE_NAME IS 'Name of the given Resource Type';</v>
+      </c>
+    </row>
+    <row r="491" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A491" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B491" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C491" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="D491" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_TYPE_DESC IS 'Description for the given Resource Type';</v>
+      </c>
+    </row>
+    <row r="492" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A492" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B492" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="C492" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="D492" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_DESC IS 'The description for the project resource';</v>
+      </c>
+    </row>
+    <row r="493" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A493" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B493" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="C493" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="D493" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>COMMENT ON COLUMN PRI_RES_PROJ_TAG_MAX_SUM_ALL_V.RES_DEMO_URL IS 'The live demonstration URL for the project resource';</v>
+      </c>
     </row>
     <row r="511" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A511" s="19"/>
@@ -13708,10 +14527,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C270"/>
+  <dimension ref="A1:C327"/>
   <sheetViews>
-    <sheetView topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="C263" sqref="C263:C266"/>
+    <sheetView topLeftCell="B295" workbookViewId="0">
+      <selection activeCell="C306" sqref="C306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16674,6 +17493,654 @@
       <c r="C270" s="18" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve">PRI_CV_USERS.LAST_MOD_BY, </v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B274" t="s">
+        <v>73</v>
+      </c>
+      <c r="C274" s="18" t="str">
+        <f t="shared" ref="C274:C327" si="10">CONCATENATE(A274, ".", B274, ", ")</f>
+        <v xml:space="preserve">PRI_PROJ_V.VC_PROJ_ID, </v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B275" t="s">
+        <v>75</v>
+      </c>
+      <c r="C275" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.PROJ_DESC, </v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B276" t="s">
+        <v>76</v>
+      </c>
+      <c r="C276" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.SSH_URL, </v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B277" t="s">
+        <v>77</v>
+      </c>
+      <c r="C277" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.HTTP_URL, </v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B278" t="s">
+        <v>78</v>
+      </c>
+      <c r="C278" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.README_URL, </v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B279" t="s">
+        <v>79</v>
+      </c>
+      <c r="C279" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.AVATAR_URL, </v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B280" t="s">
+        <v>80</v>
+      </c>
+      <c r="C280" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.PROJ_CREATE_DTM, </v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B281" t="s">
+        <v>81</v>
+      </c>
+      <c r="C281" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.PROJ_UPDATE_DTM, </v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B282" t="s">
+        <v>95</v>
+      </c>
+      <c r="C282" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.PROJ_VISIBILITY, </v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B283" t="s">
+        <v>96</v>
+      </c>
+      <c r="C283" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.PROJ_NAME_SPACE, </v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B284" t="s">
+        <v>298</v>
+      </c>
+      <c r="C284" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.DATA_SOURCE_ID, </v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B285" t="s">
+        <v>299</v>
+      </c>
+      <c r="C285" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.DATA_SOURCE_CODE, </v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B286" t="s">
+        <v>300</v>
+      </c>
+      <c r="C286" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.DATA_SOURCE_NAME, </v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B287" t="s">
+        <v>301</v>
+      </c>
+      <c r="C287" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.DATA_SOURCE_DESC, </v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B288" t="s">
+        <v>272</v>
+      </c>
+      <c r="C288" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.VC_OWNER_ID, </v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B289" t="s">
+        <v>319</v>
+      </c>
+      <c r="C289" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.OWNER_USER_ID, </v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B290" t="s">
+        <v>320</v>
+      </c>
+      <c r="C290" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.OWNER_USERNAME, </v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B291" t="s">
+        <v>321</v>
+      </c>
+      <c r="C291" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.OWNER_USER_NAME, </v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B292" t="s">
+        <v>322</v>
+      </c>
+      <c r="C292" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.OWNER_USER_EMAIL, </v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B293" t="s">
+        <v>323</v>
+      </c>
+      <c r="C293" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.OWNER_AVATAR_URL, </v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B294" t="s">
+        <v>324</v>
+      </c>
+      <c r="C294" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.OWNER_WEB_URL, </v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B295" t="s">
+        <v>273</v>
+      </c>
+      <c r="C295" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.VC_CREATOR_ID, </v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B296" t="s">
+        <v>325</v>
+      </c>
+      <c r="C296" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.CREATOR_USER_ID, </v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B297" t="s">
+        <v>326</v>
+      </c>
+      <c r="C297" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.CREATOR_USERNAME, </v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B298" t="s">
+        <v>327</v>
+      </c>
+      <c r="C298" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.CREATOR_USER_NAME, </v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B299" t="s">
+        <v>328</v>
+      </c>
+      <c r="C299" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.CREATOR_USER_EMAIL, </v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B300" t="s">
+        <v>329</v>
+      </c>
+      <c r="C300" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.CREATOR_AVATAR_URL, </v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A301" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B301" t="s">
+        <v>330</v>
+      </c>
+      <c r="C301" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.CREATOR_WEB_URL, </v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B302" t="s">
+        <v>274</v>
+      </c>
+      <c r="C302" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.VC_WEB_URL, </v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A303" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B303" t="s">
+        <v>275</v>
+      </c>
+      <c r="C303" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.VC_OPEN_ISSUES_COUNT, </v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A304" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B304" t="s">
+        <v>276</v>
+      </c>
+      <c r="C304" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.VC_COMMIT_COUNT, </v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A305" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B305" t="s">
+        <v>278</v>
+      </c>
+      <c r="C305" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.VC_REPO_SIZE, </v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A306" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B306" t="s">
+        <v>347</v>
+      </c>
+      <c r="C306" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.VC_REPO_SIZE_MB, </v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A307" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B307" t="s">
+        <v>98</v>
+      </c>
+      <c r="C307" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.CREATE_DATE, </v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A308" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B308" t="s">
+        <v>99</v>
+      </c>
+      <c r="C308" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.CREATED_BY, </v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A309" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B309" t="s">
+        <v>100</v>
+      </c>
+      <c r="C309" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.LAST_MOD_DATE, </v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A310" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B310" t="s">
+        <v>101</v>
+      </c>
+      <c r="C310" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.LAST_MOD_BY, </v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A311" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B311" t="s">
+        <v>348</v>
+      </c>
+      <c r="C311" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.PROJ_REFRESH_DATE, </v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A312" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B312" t="s">
+        <v>120</v>
+      </c>
+      <c r="C312" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_ID, </v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A313" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B313" t="s">
+        <v>121</v>
+      </c>
+      <c r="C313" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_CATEGORY, </v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A314" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B314" t="s">
+        <v>122</v>
+      </c>
+      <c r="C314" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_TAG_CONV, </v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A315" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B315" t="s">
+        <v>123</v>
+      </c>
+      <c r="C315" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_NAME, </v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A316" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B316" t="s">
+        <v>124</v>
+      </c>
+      <c r="C316" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_COLOR_CODE, </v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A317" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B317" t="s">
+        <v>125</v>
+      </c>
+      <c r="C317" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_URL, </v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A318" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B318" t="s">
+        <v>136</v>
+      </c>
+      <c r="C318" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_SCOPE_ID, </v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A319" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B319" t="s">
+        <v>143</v>
+      </c>
+      <c r="C319" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_SCOPE_CODE, </v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A320" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B320" t="s">
+        <v>144</v>
+      </c>
+      <c r="C320" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_SCOPE_NAME, </v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A321" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B321" t="s">
+        <v>145</v>
+      </c>
+      <c r="C321" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_SCOPE_DESC, </v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A322" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B322" t="s">
+        <v>135</v>
+      </c>
+      <c r="C322" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_TYPE_ID, </v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A323" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B323" t="s">
+        <v>146</v>
+      </c>
+      <c r="C323" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_TYPE_CODE, </v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A324" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B324" t="s">
+        <v>147</v>
+      </c>
+      <c r="C324" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_TYPE_NAME, </v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A325" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B325" t="s">
+        <v>148</v>
+      </c>
+      <c r="C325" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_TYPE_DESC, </v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A326" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B326" t="s">
+        <v>264</v>
+      </c>
+      <c r="C326" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_DESC, </v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A327" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B327" t="s">
+        <v>265</v>
+      </c>
+      <c r="C327" s="18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">PRI_PROJ_V.RES_DEMO_URL, </v>
       </c>
     </row>
   </sheetData>

</xml_diff>